<commit_message>
Test: Update excel to trigger action
</commit_message>
<xml_diff>
--- a/data/your_data.xlsx
+++ b/data/your_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\excel-to-html\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\product to github\horng-en\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F9A52A-1018-456F-9BA9-F056EC20DC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C01156C0-BA32-4123-8F1F-042392CC3FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5634D8D7-2CD7-4A55-9A93-AFB79072EA7D}"/>
   </bookViews>
@@ -869,10 +869,6 @@
     <t>P1112-08</t>
   </si>
   <si>
-    <t>PP(本)
-CK</t>
-  </si>
-  <si>
     <t>8-11</t>
   </si>
   <si>
@@ -1261,10 +1257,6 @@
   </si>
   <si>
     <t>PP(鐵灰)</t>
-  </si>
-  <si>
-    <t>PP(灰
-紫口)</t>
   </si>
   <si>
     <t>PP(什)</t>
@@ -1516,6 +1508,14 @@
   </si>
   <si>
     <t>拉伸強度(kgf/mc2)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PP(本)CK</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PP(灰紫口)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1927,8 +1927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3841EC-E9CE-48F0-886C-4C15E2FC0349}">
   <dimension ref="A1:P222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="B144" sqref="B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1942,52 +1942,52 @@
   <sheetData>
     <row r="1" spans="1:16" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>465</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1995,7 +1995,7 @@
         <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>64</v>
@@ -2024,7 +2024,7 @@
         <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C3" s="1">
         <v>3</v>
@@ -2059,7 +2059,7 @@
         <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C4" s="1">
         <v>0.06</v>
@@ -2820,7 +2820,7 @@
         <v>116</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C23" s="1">
         <v>0.06</v>
@@ -2855,7 +2855,7 @@
         <v>118</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C24" s="1">
         <v>0.05</v>
@@ -2890,7 +2890,7 @@
         <v>119</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C25" s="1">
         <v>0.1</v>
@@ -2925,7 +2925,7 @@
         <v>121</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C26" s="1">
         <v>0.15</v>
@@ -2960,7 +2960,7 @@
         <v>123</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C27" s="1">
         <v>0.15</v>
@@ -2995,7 +2995,7 @@
         <v>124</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C28" s="1">
         <v>0.1</v>
@@ -3045,7 +3045,7 @@
         <v>127</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C29" s="1">
         <v>0.2</v>
@@ -3095,7 +3095,7 @@
         <v>129</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C30" s="1">
         <v>0.1</v>
@@ -3130,7 +3130,7 @@
         <v>130</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C31" s="1">
         <v>0.15</v>
@@ -3165,7 +3165,7 @@
         <v>131</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C32" s="1">
         <v>0.2</v>
@@ -3203,7 +3203,7 @@
         <v>132</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C33" s="1">
         <v>0.15</v>
@@ -3238,7 +3238,7 @@
         <v>133</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C34" s="1">
         <v>0.2</v>
@@ -3273,7 +3273,7 @@
         <v>134</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C35" s="1">
         <v>0.2</v>
@@ -3373,7 +3373,7 @@
         <v>137</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C37" s="1">
         <v>0.2</v>
@@ -3423,7 +3423,7 @@
         <v>59</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C38" s="1">
         <v>0.2</v>
@@ -3473,7 +3473,7 @@
         <v>58</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C39" s="1">
         <v>0.2</v>
@@ -3523,7 +3523,7 @@
         <v>138</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C40" s="1">
         <v>0.2</v>
@@ -3573,7 +3573,7 @@
         <v>139</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C41" s="1">
         <v>0.2</v>
@@ -3623,7 +3623,7 @@
         <v>57</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C42" s="1">
         <v>0.2</v>
@@ -3673,7 +3673,7 @@
         <v>56</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C43" s="1">
         <v>0.2</v>
@@ -3718,12 +3718,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="33" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C44" s="1">
         <v>0.2</v>
@@ -3773,7 +3773,7 @@
         <v>141</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C45" s="1">
         <v>0.2</v>
@@ -3873,7 +3873,7 @@
         <v>55</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C47" s="1">
         <v>0.2</v>
@@ -3923,7 +3923,7 @@
         <v>144</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C48" s="1">
         <v>0.15</v>
@@ -3953,12 +3953,12 @@
         <v>0.95499999999999996</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="33" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>145</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C49" s="1">
         <v>0.15</v>
@@ -4003,12 +4003,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="33" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C50" s="1">
         <v>0.15</v>
@@ -4108,7 +4108,7 @@
         <v>149</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C52" s="1">
         <v>0.15</v>
@@ -4143,7 +4143,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C53" s="1">
         <v>0.2</v>
@@ -4178,7 +4178,7 @@
         <v>150</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C54" s="1">
         <v>5.5E-2</v>
@@ -4228,7 +4228,7 @@
         <v>150</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C55" s="1">
         <v>5.5E-2</v>
@@ -4278,7 +4278,7 @@
         <v>152</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C56" s="1">
         <v>0.03</v>
@@ -4328,7 +4328,7 @@
         <v>154</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C57" s="1">
         <v>0.04</v>
@@ -4373,12 +4373,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="33" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>155</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C58" s="1">
         <v>0.1</v>
@@ -4413,7 +4413,7 @@
         <v>156</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C59" s="1">
         <v>0.1</v>
@@ -4448,7 +4448,7 @@
         <v>157</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C60" s="1">
         <v>0.1</v>
@@ -4483,7 +4483,7 @@
         <v>158</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C61" s="1">
         <v>0.1</v>
@@ -4518,7 +4518,7 @@
         <v>159</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C62" s="1">
         <v>0.15</v>
@@ -4553,7 +4553,7 @@
         <v>51</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C63" s="1">
         <v>4</v>
@@ -4594,7 +4594,7 @@
         <v>50</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C64" s="1">
         <v>4</v>
@@ -4705,7 +4705,7 @@
         <v>165</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C67" s="1">
         <v>3</v>
@@ -4740,7 +4740,7 @@
         <v>166</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C68" s="1">
         <v>3</v>
@@ -4775,7 +4775,7 @@
         <v>167</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C69" s="1">
         <v>3</v>
@@ -4880,7 +4880,7 @@
         <v>172</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C72" s="1">
         <v>2</v>
@@ -4915,7 +4915,7 @@
         <v>173</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C73" s="1">
         <v>3</v>
@@ -4945,12 +4945,12 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="33" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C74" s="1">
         <v>3</v>
@@ -4988,7 +4988,7 @@
         <v>177</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C75" s="1">
         <v>3</v>
@@ -5023,7 +5023,7 @@
         <v>178</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C76" s="1">
         <v>3</v>
@@ -5058,7 +5058,7 @@
         <v>180</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C77" s="1">
         <v>10</v>
@@ -5233,7 +5233,7 @@
         <v>187</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C82" s="1">
         <v>3</v>
@@ -5259,7 +5259,7 @@
         <v>188</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C83" s="1">
         <v>7</v>
@@ -5289,12 +5289,12 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" ht="33" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>189</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C84" s="1">
         <v>6</v>
@@ -5324,12 +5324,12 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" ht="33" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>190</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C85" s="1">
         <v>0.3</v>
@@ -5359,12 +5359,12 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" ht="33" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>191</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C86" s="1">
         <v>1</v>
@@ -5394,12 +5394,12 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" ht="33" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>192</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C87" s="1">
         <v>1</v>
@@ -5434,7 +5434,7 @@
         <v>193</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C88" s="1">
         <v>35</v>
@@ -5484,7 +5484,7 @@
         <v>198</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C89" s="1">
         <v>12</v>
@@ -5534,7 +5534,7 @@
         <v>202</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C90" s="1">
         <v>25</v>
@@ -5569,7 +5569,7 @@
         <v>204</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C91" s="1">
         <v>1</v>
@@ -5604,7 +5604,7 @@
         <v>206</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C92" s="1">
         <v>0.5</v>
@@ -5639,7 +5639,7 @@
         <v>207</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C93" s="1">
         <v>3</v>
@@ -5689,7 +5689,7 @@
         <v>211</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C94" s="1">
         <v>5</v>
@@ -5718,7 +5718,7 @@
         <v>47</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C95" s="1">
         <v>5</v>
@@ -5768,7 +5768,7 @@
         <v>215</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C96" s="1">
         <v>12</v>
@@ -5812,7 +5812,7 @@
         <v>217</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C97" s="1">
         <v>15</v>
@@ -5847,7 +5847,7 @@
         <v>218</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C98" s="1">
         <v>4</v>
@@ -5894,7 +5894,7 @@
         <v>221</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C99" s="1">
         <v>8</v>
@@ -5941,7 +5941,7 @@
         <v>224</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C100" s="1">
         <v>20</v>
@@ -5976,7 +5976,7 @@
         <v>226</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C101" s="1">
         <v>5</v>
@@ -6011,7 +6011,7 @@
         <v>227</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C102" s="1">
         <v>5</v>
@@ -6052,7 +6052,7 @@
         <v>230</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C103" s="1">
         <v>4</v>
@@ -6102,7 +6102,7 @@
         <v>235</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C104" s="1">
         <v>5</v>
@@ -6137,7 +6137,7 @@
         <v>236</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C105" s="1">
         <v>5</v>
@@ -6184,7 +6184,7 @@
         <v>238</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C106" s="1">
         <v>5</v>
@@ -6219,7 +6219,7 @@
         <v>239</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C107" s="1">
         <v>8</v>
@@ -6254,7 +6254,7 @@
         <v>241</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C108" s="1">
         <v>10</v>
@@ -6292,7 +6292,7 @@
         <v>243</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C109" s="1">
         <v>1</v>
@@ -6342,7 +6342,7 @@
         <v>245</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C110" s="1">
         <v>5</v>
@@ -6377,7 +6377,7 @@
         <v>247</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C111" s="1">
         <v>5</v>
@@ -6412,7 +6412,7 @@
         <v>248</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C112" s="1">
         <v>7</v>
@@ -6450,7 +6450,7 @@
         <v>249</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C113" s="1">
         <v>5</v>
@@ -6485,7 +6485,7 @@
         <v>251</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C114" s="1">
         <v>5</v>
@@ -6520,7 +6520,7 @@
         <v>252</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C115" s="1">
         <v>3</v>
@@ -6570,7 +6570,7 @@
         <v>253</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C116" s="1">
         <v>7</v>
@@ -6608,7 +6608,7 @@
         <v>255</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C117" s="1">
         <v>6</v>
@@ -6643,7 +6643,7 @@
         <v>256</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C118" s="1">
         <v>7</v>
@@ -6678,7 +6678,7 @@
         <v>257</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C119" s="1">
         <v>10</v>
@@ -6716,7 +6716,7 @@
         <v>258</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C120" s="1">
         <v>5</v>
@@ -6766,7 +6766,7 @@
         <v>259</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C121" s="1">
         <v>6</v>
@@ -6801,7 +6801,7 @@
         <v>260</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C122" s="1">
         <v>10</v>
@@ -6836,7 +6836,7 @@
         <v>261</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C123" s="1">
         <v>8</v>
@@ -6874,7 +6874,7 @@
         <v>264</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C124" s="1">
         <v>1.5</v>
@@ -6924,7 +6924,7 @@
         <v>266</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C125" s="1">
         <v>3</v>
@@ -6950,7 +6950,7 @@
         <v>267</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>4</v>
@@ -6964,7 +6964,7 @@
         <v>268</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C127" s="1">
         <v>6</v>
@@ -7014,7 +7014,7 @@
         <v>271</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C128" s="1">
         <v>3.5</v>
@@ -7061,7 +7061,7 @@
         <v>272</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C129" s="1">
         <v>3.5</v>
@@ -7108,7 +7108,7 @@
         <v>273</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C130" s="1">
         <v>3.5</v>
@@ -7143,7 +7143,7 @@
         <v>274</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C131" s="1">
         <v>4</v>
@@ -7178,7 +7178,7 @@
         <v>275</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>276</v>
+        <v>473</v>
       </c>
       <c r="C132" s="1">
         <v>0.5</v>
@@ -7193,7 +7193,7 @@
         <v>5.99</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>5</v>
@@ -7210,10 +7210,10 @@
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C133" s="1">
         <v>18</v>
@@ -7249,7 +7249,7 @@
         <v>196</v>
       </c>
       <c r="O133" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P133" s="1" t="s">
         <v>30</v>
@@ -7257,10 +7257,10 @@
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B134" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="C134" s="1">
         <v>2</v>
@@ -7275,7 +7275,7 @@
         <v>7.84</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>11</v>
@@ -7292,10 +7292,10 @@
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C135" s="1">
         <v>2</v>
@@ -7310,7 +7310,7 @@
         <v>25.56</v>
       </c>
       <c r="G135" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H135" s="1" t="s">
         <v>5</v>
@@ -7327,10 +7327,10 @@
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H136" s="1" t="s">
         <v>4</v>
@@ -7341,10 +7341,10 @@
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C137" s="1">
         <v>18</v>
@@ -7371,7 +7371,7 @@
         <v>78</v>
       </c>
       <c r="O137" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P137" s="1" t="s">
         <v>15</v>
@@ -7379,10 +7379,10 @@
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C138" s="1">
         <v>12</v>
@@ -7414,10 +7414,10 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C139" s="1">
         <v>20</v>
@@ -7449,10 +7449,10 @@
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C140" s="1">
         <v>5</v>
@@ -7484,10 +7484,10 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C141" s="1">
         <v>13</v>
@@ -7519,10 +7519,10 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C142" s="1">
         <v>15</v>
@@ -7537,7 +7537,7 @@
         <v>5.63</v>
       </c>
       <c r="G142" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H142" s="1" t="s">
         <v>5</v>
@@ -7558,7 +7558,7 @@
         <v>147</v>
       </c>
       <c r="O142" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P142" s="1" t="s">
         <v>10</v>
@@ -7566,10 +7566,10 @@
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C143" s="1">
         <v>0.7</v>
@@ -7584,7 +7584,7 @@
         <v>7.84</v>
       </c>
       <c r="G143" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H143" s="1" t="s">
         <v>1</v>
@@ -7616,10 +7616,10 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>406</v>
+        <v>474</v>
       </c>
       <c r="C144" s="1">
         <v>4</v>
@@ -7634,7 +7634,7 @@
         <v>7.84</v>
       </c>
       <c r="G144" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H144" s="1" t="s">
         <v>2</v>
@@ -7657,10 +7657,10 @@
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C145" s="1">
         <v>4</v>
@@ -7675,7 +7675,7 @@
         <v>7.84</v>
       </c>
       <c r="G145" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H145" s="1" t="s">
         <v>2</v>
@@ -7698,10 +7698,10 @@
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C146" s="1">
         <v>3</v>
@@ -7739,10 +7739,10 @@
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B147" s="1" t="s">
         <v>299</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>300</v>
       </c>
       <c r="C147" s="1">
         <v>10</v>
@@ -7757,7 +7757,7 @@
         <v>7.84</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H147" s="1" t="s">
         <v>5</v>
@@ -7775,15 +7775,15 @@
         <v>125</v>
       </c>
       <c r="P147" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B148" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>304</v>
       </c>
       <c r="C148" s="1">
         <v>10</v>
@@ -7798,7 +7798,7 @@
         <v>7.84</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H148" s="1" t="s">
         <v>5</v>
@@ -7816,15 +7816,15 @@
         <v>125</v>
       </c>
       <c r="P148" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C149" s="1">
         <v>5</v>
@@ -7854,7 +7854,7 @@
         <v>0.91</v>
       </c>
       <c r="O149" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P149" s="1" t="s">
         <v>17</v>
@@ -7862,10 +7862,10 @@
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C150" s="1">
         <v>10</v>
@@ -7897,10 +7897,10 @@
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C151" s="1">
         <v>1.5</v>
@@ -7936,7 +7936,7 @@
         <v>27</v>
       </c>
       <c r="N151" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="O151" s="1" t="s">
         <v>265</v>
@@ -7947,10 +7947,10 @@
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H152" s="1" t="s">
         <v>4</v>
@@ -7961,10 +7961,10 @@
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H153" s="1" t="s">
         <v>4</v>
@@ -7975,10 +7975,10 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C154" s="1">
         <v>15</v>
@@ -8008,7 +8008,7 @@
         <v>0.95</v>
       </c>
       <c r="L154" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M154" s="1" t="s">
         <v>147</v>
@@ -8017,7 +8017,7 @@
         <v>262</v>
       </c>
       <c r="O154" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P154" s="1" t="s">
         <v>30</v>
@@ -8025,10 +8025,10 @@
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C155" s="1">
         <v>12</v>
@@ -8060,10 +8060,10 @@
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C156" s="1">
         <v>5</v>
@@ -8095,10 +8095,10 @@
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B157" s="1" t="s">
         <v>317</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>318</v>
       </c>
       <c r="C157" s="1">
         <v>5</v>
@@ -8130,10 +8130,10 @@
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C158" s="1">
         <v>5</v>
@@ -8165,10 +8165,10 @@
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C159" s="1">
         <v>5</v>
@@ -8200,7 +8200,7 @@
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>25</v>
@@ -8235,10 +8235,10 @@
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C161" s="1">
         <v>5</v>
@@ -8270,10 +8270,10 @@
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C162" s="1">
         <v>6</v>
@@ -8312,7 +8312,7 @@
         <v>262</v>
       </c>
       <c r="O162" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P162" s="1" t="s">
         <v>223</v>
@@ -8320,10 +8320,10 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C163" s="1">
         <v>5</v>
@@ -8353,7 +8353,7 @@
         <v>0.94</v>
       </c>
       <c r="O163" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P163" s="1" t="s">
         <v>17</v>
@@ -8361,10 +8361,10 @@
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C164" s="1">
         <v>5</v>
@@ -8394,7 +8394,7 @@
         <v>0.94</v>
       </c>
       <c r="O164" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P164" s="1" t="s">
         <v>17</v>
@@ -8402,10 +8402,10 @@
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C165" s="1">
         <v>5</v>
@@ -8435,7 +8435,7 @@
         <v>0.94</v>
       </c>
       <c r="O165" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P165" s="1" t="s">
         <v>17</v>
@@ -8443,10 +8443,10 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C166" s="1">
         <v>12</v>
@@ -8478,10 +8478,10 @@
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C167" s="1">
         <v>12</v>
@@ -8513,10 +8513,10 @@
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C168" s="1">
         <v>18</v>
@@ -8543,7 +8543,7 @@
         <v>78</v>
       </c>
       <c r="O168" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P168" s="1" t="s">
         <v>15</v>
@@ -8551,10 +8551,10 @@
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B169" s="1" t="s">
         <v>330</v>
-      </c>
-      <c r="B169" s="1" t="s">
-        <v>331</v>
       </c>
       <c r="C169" s="1">
         <v>7</v>
@@ -8586,10 +8586,10 @@
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C170" s="1">
         <v>10</v>
@@ -8621,10 +8621,10 @@
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C171" s="1">
         <v>7</v>
@@ -8656,10 +8656,10 @@
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C172" s="1">
         <v>5</v>
@@ -8691,10 +8691,10 @@
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C173" s="1">
         <v>15</v>
@@ -8709,7 +8709,7 @@
         <v>5.63</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H173" s="1" t="s">
         <v>5</v>
@@ -8730,7 +8730,7 @@
         <v>147</v>
       </c>
       <c r="O173" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P173" s="1" t="s">
         <v>10</v>
@@ -8738,10 +8738,10 @@
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C174" s="1">
         <v>4</v>
@@ -8771,7 +8771,7 @@
         <v>0.94</v>
       </c>
       <c r="O174" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P174" s="1" t="s">
         <v>30</v>
@@ -8779,10 +8779,10 @@
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C175" s="1">
         <v>4</v>
@@ -8812,7 +8812,7 @@
         <v>0.94</v>
       </c>
       <c r="O175" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P175" s="1" t="s">
         <v>30</v>
@@ -8820,7 +8820,7 @@
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>24</v>
@@ -8855,7 +8855,7 @@
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>24</v>
@@ -8890,7 +8890,7 @@
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>24</v>
@@ -8925,10 +8925,10 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B179" s="1" t="s">
         <v>341</v>
-      </c>
-      <c r="B179" s="1" t="s">
-        <v>342</v>
       </c>
       <c r="C179" s="1">
         <v>4</v>
@@ -8967,7 +8967,7 @@
         <v>262</v>
       </c>
       <c r="O179" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P179" s="1" t="s">
         <v>223</v>
@@ -8975,10 +8975,10 @@
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B180" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="B180" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="C180" s="1">
         <v>10</v>
@@ -8993,7 +8993,7 @@
         <v>7.84</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H180" s="1" t="s">
         <v>5</v>
@@ -9011,15 +9011,15 @@
         <v>125</v>
       </c>
       <c r="P180" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B181" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="B181" s="1" t="s">
-        <v>346</v>
       </c>
       <c r="C181" s="1">
         <v>10</v>
@@ -9034,7 +9034,7 @@
         <v>7.84</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H181" s="1" t="s">
         <v>5</v>
@@ -9052,15 +9052,15 @@
         <v>125</v>
       </c>
       <c r="P181" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C182" s="1">
         <v>12</v>
@@ -9092,10 +9092,10 @@
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C183" s="1">
         <v>0.7</v>
@@ -9110,7 +9110,7 @@
         <v>7.84</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H183" s="1" t="s">
         <v>1</v>
@@ -9139,10 +9139,10 @@
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C184" s="1">
         <v>15</v>
@@ -9174,10 +9174,10 @@
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C185" s="1">
         <v>12</v>
@@ -9209,10 +9209,10 @@
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C186" s="1">
         <v>18</v>
@@ -9239,7 +9239,7 @@
         <v>78</v>
       </c>
       <c r="O186" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P186" s="1" t="s">
         <v>15</v>
@@ -9247,10 +9247,10 @@
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C187" s="1">
         <v>25</v>
@@ -9280,15 +9280,15 @@
         <v>0.93</v>
       </c>
       <c r="P187" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C188" s="1">
         <v>12</v>
@@ -9320,10 +9320,10 @@
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C189" s="1">
         <v>5</v>
@@ -9355,10 +9355,10 @@
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C190" s="1">
         <v>5</v>
@@ -9390,10 +9390,10 @@
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C191" s="1">
         <v>15</v>
@@ -9408,7 +9408,7 @@
         <v>5.63</v>
       </c>
       <c r="G191" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H191" s="1" t="s">
         <v>5</v>
@@ -9429,7 +9429,7 @@
         <v>147</v>
       </c>
       <c r="O191" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P191" s="1" t="s">
         <v>10</v>
@@ -9437,10 +9437,10 @@
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C192" s="1">
         <v>5</v>
@@ -9472,10 +9472,10 @@
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C193" s="1">
         <v>4</v>
@@ -9507,10 +9507,10 @@
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C194" s="1">
         <v>5</v>
@@ -9542,10 +9542,10 @@
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C195" s="1">
         <v>5</v>
@@ -9575,7 +9575,7 @@
         <v>0.94</v>
       </c>
       <c r="O195" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P195" s="1" t="s">
         <v>17</v>
@@ -9586,7 +9586,7 @@
         <v>18</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C196" s="1">
         <v>5</v>
@@ -9616,7 +9616,7 @@
         <v>0.94</v>
       </c>
       <c r="O196" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P196" s="1" t="s">
         <v>17</v>
@@ -9624,10 +9624,10 @@
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C197" s="1">
         <v>5</v>
@@ -9659,7 +9659,7 @@
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>16</v>
@@ -9694,10 +9694,10 @@
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C199" s="1">
         <v>4</v>
@@ -9729,10 +9729,10 @@
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C200" s="1">
         <v>5</v>
@@ -9764,10 +9764,10 @@
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C201" s="1">
         <v>18</v>
@@ -9794,7 +9794,7 @@
         <v>78</v>
       </c>
       <c r="O201" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="P201" s="1" t="s">
         <v>15</v>
@@ -9802,10 +9802,10 @@
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C202" s="1">
         <v>5</v>
@@ -9837,10 +9837,10 @@
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C203" s="1">
         <v>5</v>
@@ -9872,10 +9872,10 @@
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C204" s="1">
         <v>2</v>
@@ -9907,10 +9907,10 @@
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C205" s="1">
         <v>12</v>
@@ -9942,10 +9942,10 @@
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C206" s="1">
         <v>5</v>
@@ -9978,15 +9978,15 @@
         <v>200</v>
       </c>
       <c r="P206" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C207" s="1">
         <v>25</v>
@@ -10018,10 +10018,10 @@
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C208" s="1">
         <v>20</v>
@@ -10053,10 +10053,10 @@
     </row>
     <row r="209" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C209" s="1">
         <v>6</v>
@@ -10086,7 +10086,7 @@
         <v>0.98</v>
       </c>
       <c r="O209" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="P209" s="1" t="s">
         <v>10</v>
@@ -10094,10 +10094,10 @@
     </row>
     <row r="210" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C210" s="1">
         <v>1</v>
@@ -10129,10 +10129,10 @@
     </row>
     <row r="211" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C211" s="1">
         <v>3</v>
@@ -10164,10 +10164,10 @@
     </row>
     <row r="212" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C212" s="1">
         <v>7</v>
@@ -10202,7 +10202,7 @@
         <v>12</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C213" s="1">
         <v>7</v>
@@ -10234,10 +10234,10 @@
     </row>
     <row r="214" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C214" s="1">
         <v>5</v>
@@ -10269,10 +10269,10 @@
     </row>
     <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B215" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>383</v>
       </c>
       <c r="C215" s="1">
         <v>15</v>
@@ -10287,7 +10287,7 @@
         <v>5.63</v>
       </c>
       <c r="G215" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H215" s="1" t="s">
         <v>5</v>
@@ -10308,7 +10308,7 @@
         <v>147</v>
       </c>
       <c r="O215" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P215" s="1" t="s">
         <v>10</v>
@@ -10316,10 +10316,10 @@
     </row>
     <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C216" s="1">
         <v>4</v>
@@ -10357,10 +10357,10 @@
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C217" s="1">
         <v>4</v>
@@ -10392,10 +10392,10 @@
     </row>
     <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C218" s="1">
         <v>6</v>
@@ -10434,7 +10434,7 @@
         <v>262</v>
       </c>
       <c r="O218" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P218" s="1" t="s">
         <v>223</v>
@@ -10442,10 +10442,10 @@
     </row>
     <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C219" s="1">
         <v>10</v>
@@ -10460,7 +10460,7 @@
         <v>7.84</v>
       </c>
       <c r="G219" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H219" s="1" t="s">
         <v>5</v>
@@ -10478,15 +10478,15 @@
         <v>125</v>
       </c>
       <c r="P219" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H220" s="1" t="s">
         <v>4</v>
@@ -10497,10 +10497,10 @@
     </row>
     <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C221" s="1">
         <v>6</v>
@@ -10515,7 +10515,7 @@
         <v>20.88</v>
       </c>
       <c r="G221" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H221" s="1" t="s">
         <v>3</v>
@@ -10530,12 +10530,12 @@
         <v>0.93</v>
       </c>
       <c r="P221" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="222" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B222" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C222" s="1">
         <v>30</v>

</xml_diff>